<commit_message>
Saving as image (continued)
</commit_message>
<xml_diff>
--- a/esc_data.xlsx
+++ b/esc_data.xlsx
@@ -43840,6 +43840,12 @@
           <t>zauvijekvolimte</t>
         </is>
       </c>
+      <c r="I1073" t="n">
+        <v>0</v>
+      </c>
+      <c r="J1073" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="1074">
       <c r="A1074" s="9" t="inlineStr">
@@ -43882,6 +43888,12 @@
           <t>thefireinyoureyes</t>
         </is>
       </c>
+      <c r="I1074" t="n">
+        <v>1</v>
+      </c>
+      <c r="J1074" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="1075">
       <c r="A1075" s="9" t="inlineStr">
@@ -43924,6 +43936,12 @@
           <t>letosvet</t>
         </is>
       </c>
+      <c r="I1075" t="n">
+        <v>2</v>
+      </c>
+      <c r="J1075" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="1076">
       <c r="A1076" s="9" t="inlineStr">
@@ -43966,6 +43984,12 @@
           <t>acenturyoflove</t>
         </is>
       </c>
+      <c r="I1076" t="n">
+        <v>3</v>
+      </c>
+      <c r="J1076" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="1077">
       <c r="A1077" s="9" t="inlineStr">
@@ -44008,6 +44032,12 @@
           <t>complice</t>
         </is>
       </c>
+      <c r="I1077" t="n">
+        <v>4</v>
+      </c>
+      <c r="J1077" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="1078">
       <c r="A1078" s="9" t="inlineStr">
@@ -44050,6 +44080,12 @@
           <t>ojulissi</t>
         </is>
       </c>
+      <c r="I1078" t="n">
+        <v>5</v>
+      </c>
+      <c r="J1078" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="1079">
       <c r="A1079" s="9" t="inlineStr">
@@ -44092,6 +44128,12 @@
           <t>dayafterday</t>
         </is>
       </c>
+      <c r="I1079" t="n">
+        <v>6</v>
+      </c>
+      <c r="J1079" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="1080">
       <c r="A1080" s="9" t="inlineStr">
@@ -44134,6 +44176,12 @@
           <t>vragnajvzame</t>
         </is>
       </c>
+      <c r="I1080" t="n">
+        <v>7</v>
+      </c>
+      <c r="J1080" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="1081">
       <c r="A1081" s="9" t="inlineStr">
@@ -44176,6 +44224,12 @@
           <t>holdonbestrong</t>
         </is>
       </c>
+      <c r="I1081" t="n">
+        <v>8</v>
+      </c>
+      <c r="J1081" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="1082">
       <c r="A1082" s="9" t="inlineStr">
@@ -44218,6 +44272,12 @@
           <t>forlife</t>
         </is>
       </c>
+      <c r="I1082" t="n">
+        <v>9</v>
+      </c>
+      <c r="J1082" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="1083">
       <c r="A1083" s="9" t="inlineStr">
@@ -44260,6 +44320,12 @@
           <t>irelandedouzepointe</t>
         </is>
       </c>
+      <c r="I1083" t="n">
+        <v>10</v>
+      </c>
+      <c r="J1083" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="1084">
       <c r="A1084" s="9" t="inlineStr">
@@ -44302,6 +44368,12 @@
           <t>casanova</t>
         </is>
       </c>
+      <c r="I1084" t="n">
+        <v>11</v>
+      </c>
+      <c r="J1084" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="1085">
       <c r="A1085" s="9" t="inlineStr">
@@ -44344,6 +44416,12 @@
           <t>pokusaj</t>
         </is>
       </c>
+      <c r="I1085" t="n">
+        <v>12</v>
+      </c>
+      <c r="J1085" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="1086">
       <c r="A1086" s="9" t="inlineStr">
@@ -44386,6 +44464,12 @@
           <t>qeleqele</t>
         </is>
       </c>
+      <c r="I1086" t="n">
+        <v>13</v>
+      </c>
+      <c r="J1086" t="n">
+        <v>13</v>
+      </c>
     </row>
     <row r="1087">
       <c r="A1087" s="9" t="inlineStr">
@@ -44428,6 +44512,12 @@
           <t>yourheartbelongstome</t>
         </is>
       </c>
+      <c r="I1087" t="n">
+        <v>14</v>
+      </c>
+      <c r="J1087" t="n">
+        <v>14</v>
+      </c>
     </row>
     <row r="1088">
       <c r="A1088" s="9" t="inlineStr">
@@ -44470,6 +44560,12 @@
           <t>missamiehetratsastaa</t>
         </is>
       </c>
+      <c r="I1088" t="n">
+        <v>15</v>
+      </c>
+      <c r="J1088" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="1089">
       <c r="A1089" s="9" t="inlineStr">
@@ -44512,6 +44608,12 @@
           <t>peomarginedelume</t>
         </is>
       </c>
+      <c r="I1089" t="n">
+        <v>16</v>
+      </c>
+      <c r="J1089" t="n">
+        <v>16</v>
+      </c>
     </row>
     <row r="1090">
       <c r="A1090" s="9" t="inlineStr">
@@ -44554,6 +44656,12 @@
           <t>believe</t>
         </is>
       </c>
+      <c r="I1090" t="n">
+        <v>17</v>
+      </c>
+      <c r="J1090" t="n">
+        <v>17</v>
+      </c>
     </row>
     <row r="1091">
       <c r="A1091" s="9" t="inlineStr">
@@ -44596,6 +44704,12 @@
           <t>secretcombination</t>
         </is>
       </c>
+      <c r="I1091" t="n">
+        <v>18</v>
+      </c>
+      <c r="J1091" t="n">
+        <v>18</v>
+      </c>
     </row>
     <row r="1092">
       <c r="A1092" s="9" t="inlineStr">
@@ -44638,6 +44752,12 @@
           <t>thisismylife</t>
         </is>
       </c>
+      <c r="I1092" t="n">
+        <v>19</v>
+      </c>
+      <c r="J1092" t="n">
+        <v>19</v>
+      </c>
     </row>
     <row r="1093">
       <c r="A1093" s="9" t="inlineStr">
@@ -44680,6 +44800,12 @@
           <t>hero</t>
         </is>
       </c>
+      <c r="I1093" t="n">
+        <v>20</v>
+      </c>
+      <c r="J1093" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="1094">
       <c r="A1094" s="9" t="inlineStr">
@@ -44722,6 +44848,12 @@
           <t>deli</t>
         </is>
       </c>
+      <c r="I1094" t="n">
+        <v>21</v>
+      </c>
+      <c r="J1094" t="n">
+        <v>21</v>
+      </c>
     </row>
     <row r="1095">
       <c r="A1095" s="9" t="inlineStr">
@@ -44764,6 +44896,12 @@
           <t>shadylady</t>
         </is>
       </c>
+      <c r="I1095" t="n">
+        <v>22</v>
+      </c>
+      <c r="J1095" t="n">
+        <v>22</v>
+      </c>
     </row>
     <row r="1096">
       <c r="A1096" s="9" t="inlineStr">
@@ -44806,6 +44944,12 @@
           <t>nomadsinthenight</t>
         </is>
       </c>
+      <c r="I1096" t="n">
+        <v>23</v>
+      </c>
+      <c r="J1096" t="n">
+        <v>23</v>
+      </c>
     </row>
     <row r="1097">
       <c r="A1097" s="9" t="inlineStr">
@@ -44848,6 +44992,12 @@
           <t>zemrenelamepeng</t>
         </is>
       </c>
+      <c r="I1097" t="n">
+        <v>24</v>
+      </c>
+      <c r="J1097" t="n">
+        <v>24</v>
+      </c>
     </row>
     <row r="1098">
       <c r="A1098" s="9" t="inlineStr">
@@ -44890,6 +45040,12 @@
           <t>erastupendo</t>
         </is>
       </c>
+      <c r="I1098" t="n">
+        <v>25</v>
+      </c>
+      <c r="J1098" t="n">
+        <v>25</v>
+      </c>
     </row>
     <row r="1099">
       <c r="A1099" s="9" t="inlineStr">
@@ -44932,6 +45088,12 @@
           <t>havesomefun</t>
         </is>
       </c>
+      <c r="I1099" t="n">
+        <v>26</v>
+      </c>
+      <c r="J1099" t="n">
+        <v>26</v>
+      </c>
     </row>
     <row r="1100">
       <c r="A1100" s="9" t="inlineStr">
@@ -44974,6 +45136,12 @@
           <t>hastalavista</t>
         </is>
       </c>
+      <c r="I1100" t="n">
+        <v>27</v>
+      </c>
+      <c r="J1100" t="n">
+        <v>27</v>
+      </c>
     </row>
     <row r="1101">
       <c r="A1101" s="9" t="inlineStr">
@@ -45016,6 +45184,12 @@
           <t>wolvesofthesea</t>
         </is>
       </c>
+      <c r="I1101" t="n">
+        <v>28</v>
+      </c>
+      <c r="J1101" t="n">
+        <v>28</v>
+      </c>
     </row>
     <row r="1102">
       <c r="A1102" s="9" t="inlineStr">
@@ -45058,6 +45232,12 @@
           <t>romanca</t>
         </is>
       </c>
+      <c r="I1102" t="n">
+        <v>29</v>
+      </c>
+      <c r="J1102" t="n">
+        <v>29</v>
+      </c>
     </row>
     <row r="1103">
       <c r="A1103" s="9" t="inlineStr">
@@ -45100,6 +45280,12 @@
           <t>djtakemeaway</t>
         </is>
       </c>
+      <c r="I1103" t="n">
+        <v>30</v>
+      </c>
+      <c r="J1103" t="n">
+        <v>30</v>
+      </c>
     </row>
     <row r="1104">
       <c r="A1104" s="9" t="inlineStr">
@@ -45142,6 +45328,12 @@
           <t>allnightlong</t>
         </is>
       </c>
+      <c r="I1104" t="n">
+        <v>31</v>
+      </c>
+      <c r="J1104" t="n">
+        <v>31</v>
+      </c>
     </row>
     <row r="1105">
       <c r="A1105" s="9" t="inlineStr">
@@ -45184,6 +45376,12 @@
           <t>peacewillcome</t>
         </is>
       </c>
+      <c r="I1105" t="n">
+        <v>32</v>
+      </c>
+      <c r="J1105" t="n">
+        <v>32</v>
+      </c>
     </row>
     <row r="1106">
       <c r="A1106" s="9" t="inlineStr">
@@ -45226,6 +45424,12 @@
           <t>candlelight</t>
         </is>
       </c>
+      <c r="I1106" t="n">
+        <v>33</v>
+      </c>
+      <c r="J1106" t="n">
+        <v>33</v>
+      </c>
     </row>
     <row r="1107">
       <c r="A1107" s="9" t="inlineStr">
@@ -45268,6 +45472,12 @@
           <t>vodka</t>
         </is>
       </c>
+      <c r="I1107" t="n">
+        <v>34</v>
+      </c>
+      <c r="J1107" t="n">
+        <v>34</v>
+      </c>
     </row>
     <row r="1108">
       <c r="A1108" s="9" t="inlineStr">
@@ -45310,6 +45520,12 @@
           <t>femmefatale</t>
         </is>
       </c>
+      <c r="I1108" t="n">
+        <v>35</v>
+      </c>
+      <c r="J1108" t="n">
+        <v>35</v>
+      </c>
     </row>
     <row r="1109">
       <c r="A1109" s="9" t="inlineStr">
@@ -45352,6 +45568,12 @@
           <t>letmeloveyou</t>
         </is>
       </c>
+      <c r="I1109" t="n">
+        <v>36</v>
+      </c>
+      <c r="J1109" t="n">
+        <v>36</v>
+      </c>
     </row>
     <row r="1110">
       <c r="A1110" s="9" t="inlineStr">
@@ -45394,6 +45616,12 @@
           <t>senhoradomarnegrasaguas|senhoradomar</t>
         </is>
       </c>
+      <c r="I1110" t="n">
+        <v>37</v>
+      </c>
+      <c r="J1110" t="n">
+        <v>37</v>
+      </c>
     </row>
     <row r="1111">
       <c r="A1111" s="9" t="inlineStr">
@@ -45434,6 +45662,12 @@
           <t>evenif</t>
         </is>
       </c>
+      <c r="I1111" t="n">
+        <v>38</v>
+      </c>
+      <c r="J1111" t="n">
+        <v>38</v>
+      </c>
     </row>
     <row r="1112">
       <c r="A1112" s="9" t="inlineStr">
@@ -45474,6 +45708,12 @@
           <t>disappear</t>
         </is>
       </c>
+      <c r="I1112" t="n">
+        <v>39</v>
+      </c>
+      <c r="J1112" t="n">
+        <v>39</v>
+      </c>
     </row>
     <row r="1113">
       <c r="A1113" s="9" t="inlineStr">
@@ -45514,6 +45754,12 @@
           <t>divine</t>
         </is>
       </c>
+      <c r="I1113" t="n">
+        <v>40</v>
+      </c>
+      <c r="J1113" t="n">
+        <v>40</v>
+      </c>
     </row>
     <row r="1114">
       <c r="A1114" s="9" t="inlineStr">
@@ -45554,6 +45800,12 @@
           <t>bailaelchikichiki</t>
         </is>
       </c>
+      <c r="I1114" t="n">
+        <v>41</v>
+      </c>
+      <c r="J1114" t="n">
+        <v>41</v>
+      </c>
     </row>
     <row r="1115" ht="15.75" customHeight="1" thickBot="1">
       <c r="A1115" s="11" t="inlineStr">
@@ -45593,6 +45845,12 @@
         <is>
           <t>oro</t>
         </is>
+      </c>
+      <c r="I1115" t="n">
+        <v>42</v>
+      </c>
+      <c r="J1115" t="n">
+        <v>42</v>
       </c>
     </row>
     <row r="1116">

</xml_diff>

<commit_message>
Fully implemented saving as image
</commit_message>
<xml_diff>
--- a/esc_data.xlsx
+++ b/esc_data.xlsx
@@ -43846,6 +43846,9 @@
       <c r="J1073" t="n">
         <v>0</v>
       </c>
+      <c r="K1073" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="1074">
       <c r="A1074" s="9" t="inlineStr">
@@ -43894,6 +43897,9 @@
       <c r="J1074" t="n">
         <v>1</v>
       </c>
+      <c r="K1074" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="1075">
       <c r="A1075" s="9" t="inlineStr">
@@ -43942,6 +43948,9 @@
       <c r="J1075" t="n">
         <v>2</v>
       </c>
+      <c r="K1075" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="1076">
       <c r="A1076" s="9" t="inlineStr">
@@ -43990,6 +43999,9 @@
       <c r="J1076" t="n">
         <v>3</v>
       </c>
+      <c r="K1076" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="1077">
       <c r="A1077" s="9" t="inlineStr">
@@ -44038,6 +44050,9 @@
       <c r="J1077" t="n">
         <v>4</v>
       </c>
+      <c r="K1077" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="1078">
       <c r="A1078" s="9" t="inlineStr">
@@ -44086,6 +44101,9 @@
       <c r="J1078" t="n">
         <v>5</v>
       </c>
+      <c r="K1078" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="1079">
       <c r="A1079" s="9" t="inlineStr">
@@ -44134,6 +44152,9 @@
       <c r="J1079" t="n">
         <v>6</v>
       </c>
+      <c r="K1079" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="1080">
       <c r="A1080" s="9" t="inlineStr">
@@ -44182,6 +44203,9 @@
       <c r="J1080" t="n">
         <v>7</v>
       </c>
+      <c r="K1080" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="1081">
       <c r="A1081" s="9" t="inlineStr">
@@ -44230,6 +44254,9 @@
       <c r="J1081" t="n">
         <v>8</v>
       </c>
+      <c r="K1081" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="1082">
       <c r="A1082" s="9" t="inlineStr">
@@ -44278,6 +44305,9 @@
       <c r="J1082" t="n">
         <v>9</v>
       </c>
+      <c r="K1082" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="1083">
       <c r="A1083" s="9" t="inlineStr">
@@ -44326,6 +44356,9 @@
       <c r="J1083" t="n">
         <v>10</v>
       </c>
+      <c r="K1083" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="1084">
       <c r="A1084" s="9" t="inlineStr">
@@ -44374,6 +44407,9 @@
       <c r="J1084" t="n">
         <v>11</v>
       </c>
+      <c r="K1084" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="1085">
       <c r="A1085" s="9" t="inlineStr">
@@ -44422,6 +44458,9 @@
       <c r="J1085" t="n">
         <v>12</v>
       </c>
+      <c r="K1085" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="1086">
       <c r="A1086" s="9" t="inlineStr">
@@ -44470,6 +44509,9 @@
       <c r="J1086" t="n">
         <v>13</v>
       </c>
+      <c r="K1086" t="n">
+        <v>13</v>
+      </c>
     </row>
     <row r="1087">
       <c r="A1087" s="9" t="inlineStr">
@@ -44518,6 +44560,9 @@
       <c r="J1087" t="n">
         <v>14</v>
       </c>
+      <c r="K1087" t="n">
+        <v>14</v>
+      </c>
     </row>
     <row r="1088">
       <c r="A1088" s="9" t="inlineStr">
@@ -44566,6 +44611,9 @@
       <c r="J1088" t="n">
         <v>15</v>
       </c>
+      <c r="K1088" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="1089">
       <c r="A1089" s="9" t="inlineStr">
@@ -44614,6 +44662,9 @@
       <c r="J1089" t="n">
         <v>16</v>
       </c>
+      <c r="K1089" t="n">
+        <v>16</v>
+      </c>
     </row>
     <row r="1090">
       <c r="A1090" s="9" t="inlineStr">
@@ -44662,6 +44713,9 @@
       <c r="J1090" t="n">
         <v>17</v>
       </c>
+      <c r="K1090" t="n">
+        <v>17</v>
+      </c>
     </row>
     <row r="1091">
       <c r="A1091" s="9" t="inlineStr">
@@ -44710,6 +44764,9 @@
       <c r="J1091" t="n">
         <v>18</v>
       </c>
+      <c r="K1091" t="n">
+        <v>18</v>
+      </c>
     </row>
     <row r="1092">
       <c r="A1092" s="9" t="inlineStr">
@@ -44758,6 +44815,9 @@
       <c r="J1092" t="n">
         <v>19</v>
       </c>
+      <c r="K1092" t="n">
+        <v>19</v>
+      </c>
     </row>
     <row r="1093">
       <c r="A1093" s="9" t="inlineStr">
@@ -44806,6 +44866,9 @@
       <c r="J1093" t="n">
         <v>20</v>
       </c>
+      <c r="K1093" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="1094">
       <c r="A1094" s="9" t="inlineStr">
@@ -44854,6 +44917,9 @@
       <c r="J1094" t="n">
         <v>21</v>
       </c>
+      <c r="K1094" t="n">
+        <v>21</v>
+      </c>
     </row>
     <row r="1095">
       <c r="A1095" s="9" t="inlineStr">
@@ -44902,6 +44968,9 @@
       <c r="J1095" t="n">
         <v>22</v>
       </c>
+      <c r="K1095" t="n">
+        <v>22</v>
+      </c>
     </row>
     <row r="1096">
       <c r="A1096" s="9" t="inlineStr">
@@ -44950,6 +45019,9 @@
       <c r="J1096" t="n">
         <v>23</v>
       </c>
+      <c r="K1096" t="n">
+        <v>23</v>
+      </c>
     </row>
     <row r="1097">
       <c r="A1097" s="9" t="inlineStr">
@@ -44998,6 +45070,9 @@
       <c r="J1097" t="n">
         <v>24</v>
       </c>
+      <c r="K1097" t="n">
+        <v>24</v>
+      </c>
     </row>
     <row r="1098">
       <c r="A1098" s="9" t="inlineStr">
@@ -45046,6 +45121,9 @@
       <c r="J1098" t="n">
         <v>25</v>
       </c>
+      <c r="K1098" t="n">
+        <v>25</v>
+      </c>
     </row>
     <row r="1099">
       <c r="A1099" s="9" t="inlineStr">
@@ -45094,6 +45172,9 @@
       <c r="J1099" t="n">
         <v>26</v>
       </c>
+      <c r="K1099" t="n">
+        <v>26</v>
+      </c>
     </row>
     <row r="1100">
       <c r="A1100" s="9" t="inlineStr">
@@ -45142,6 +45223,9 @@
       <c r="J1100" t="n">
         <v>27</v>
       </c>
+      <c r="K1100" t="n">
+        <v>27</v>
+      </c>
     </row>
     <row r="1101">
       <c r="A1101" s="9" t="inlineStr">
@@ -45190,6 +45274,9 @@
       <c r="J1101" t="n">
         <v>28</v>
       </c>
+      <c r="K1101" t="n">
+        <v>28</v>
+      </c>
     </row>
     <row r="1102">
       <c r="A1102" s="9" t="inlineStr">
@@ -45238,6 +45325,9 @@
       <c r="J1102" t="n">
         <v>29</v>
       </c>
+      <c r="K1102" t="n">
+        <v>29</v>
+      </c>
     </row>
     <row r="1103">
       <c r="A1103" s="9" t="inlineStr">
@@ -45286,6 +45376,9 @@
       <c r="J1103" t="n">
         <v>30</v>
       </c>
+      <c r="K1103" t="n">
+        <v>30</v>
+      </c>
     </row>
     <row r="1104">
       <c r="A1104" s="9" t="inlineStr">
@@ -45334,6 +45427,9 @@
       <c r="J1104" t="n">
         <v>31</v>
       </c>
+      <c r="K1104" t="n">
+        <v>31</v>
+      </c>
     </row>
     <row r="1105">
       <c r="A1105" s="9" t="inlineStr">
@@ -45382,6 +45478,9 @@
       <c r="J1105" t="n">
         <v>32</v>
       </c>
+      <c r="K1105" t="n">
+        <v>32</v>
+      </c>
     </row>
     <row r="1106">
       <c r="A1106" s="9" t="inlineStr">
@@ -45430,6 +45529,9 @@
       <c r="J1106" t="n">
         <v>33</v>
       </c>
+      <c r="K1106" t="n">
+        <v>33</v>
+      </c>
     </row>
     <row r="1107">
       <c r="A1107" s="9" t="inlineStr">
@@ -45478,6 +45580,9 @@
       <c r="J1107" t="n">
         <v>34</v>
       </c>
+      <c r="K1107" t="n">
+        <v>34</v>
+      </c>
     </row>
     <row r="1108">
       <c r="A1108" s="9" t="inlineStr">
@@ -45526,6 +45631,9 @@
       <c r="J1108" t="n">
         <v>35</v>
       </c>
+      <c r="K1108" t="n">
+        <v>35</v>
+      </c>
     </row>
     <row r="1109">
       <c r="A1109" s="9" t="inlineStr">
@@ -45574,6 +45682,9 @@
       <c r="J1109" t="n">
         <v>36</v>
       </c>
+      <c r="K1109" t="n">
+        <v>36</v>
+      </c>
     </row>
     <row r="1110">
       <c r="A1110" s="9" t="inlineStr">
@@ -45622,6 +45733,9 @@
       <c r="J1110" t="n">
         <v>37</v>
       </c>
+      <c r="K1110" t="n">
+        <v>37</v>
+      </c>
     </row>
     <row r="1111">
       <c r="A1111" s="9" t="inlineStr">
@@ -45668,6 +45782,9 @@
       <c r="J1111" t="n">
         <v>38</v>
       </c>
+      <c r="K1111" t="n">
+        <v>38</v>
+      </c>
     </row>
     <row r="1112">
       <c r="A1112" s="9" t="inlineStr">
@@ -45714,6 +45831,9 @@
       <c r="J1112" t="n">
         <v>39</v>
       </c>
+      <c r="K1112" t="n">
+        <v>39</v>
+      </c>
     </row>
     <row r="1113">
       <c r="A1113" s="9" t="inlineStr">
@@ -45760,6 +45880,9 @@
       <c r="J1113" t="n">
         <v>40</v>
       </c>
+      <c r="K1113" t="n">
+        <v>40</v>
+      </c>
     </row>
     <row r="1114">
       <c r="A1114" s="9" t="inlineStr">
@@ -45806,6 +45929,9 @@
       <c r="J1114" t="n">
         <v>41</v>
       </c>
+      <c r="K1114" t="n">
+        <v>41</v>
+      </c>
     </row>
     <row r="1115" ht="15.75" customHeight="1" thickBot="1">
       <c r="A1115" s="11" t="inlineStr">
@@ -45850,6 +45976,9 @@
         <v>42</v>
       </c>
       <c r="J1115" t="n">
+        <v>42</v>
+      </c>
+      <c r="K1115" t="n">
         <v>42</v>
       </c>
     </row>

</xml_diff>